<commit_message>
Actualizacion de la semana
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_Prices_LowOil_R5.xlsx
+++ b/SuppXLS/Scen_Prices_LowOil_R5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JULIAN\Music\TIMES-UIS-v1-Nov\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4B390E8-9597-4299-A667-DF8B4A7D6203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5438AE9-6ACB-41E9-A2CF-1E7F872C842D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23555,8 +23555,8 @@
   </sheetPr>
   <dimension ref="A1:AO291"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="L217" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q244" sqref="Q244:Q251"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F54" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K75" sqref="K75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26400,7 +26400,7 @@
         <v>73</v>
       </c>
       <c r="J75">
-        <v>22.631883642110068</v>
+        <v>22.6318836421101</v>
       </c>
       <c r="K75">
         <v>22.339540412044375</v>
@@ -26978,7 +26978,7 @@
       </c>
       <c r="J93" s="25">
         <f t="shared" si="10"/>
-        <v>21.450884058013838</v>
+        <v>21.450884058013866</v>
       </c>
       <c r="K93" s="25">
         <f t="shared" si="10"/>
@@ -28368,7 +28368,7 @@
       </c>
       <c r="O188" cm="1">
         <f t="array" ref="O188:O195">+TRANSPOSE(J93:Q93)</f>
-        <v>21.450884058013838</v>
+        <v>21.450884058013866</v>
       </c>
       <c r="Q188" t="s">
         <v>113</v>
@@ -30247,7 +30247,7 @@
       <c r="N284" s="38"/>
       <c r="O284" s="38">
         <f t="shared" si="22"/>
-        <v>22.523428260914528</v>
+        <v>22.52342826091456</v>
       </c>
       <c r="P284" s="38"/>
       <c r="Q284" s="38" t="str">

</xml_diff>